<commit_message>
Added finalized production files for v0.1r1.
</commit_message>
<xml_diff>
--- a/driver_cplex_rp2040/production/ver0p1_rev1/BOM_JLCPCB_cplex_rp2040_v0p1_r1.xlsx
+++ b/driver_cplex_rp2040/production/ver0p1_rev1/BOM_JLCPCB_cplex_rp2040_v0p1_r1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="78">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -263,7 +263,7 @@
     <t xml:space="preserve">through-hole</t>
   </si>
   <si>
-    <t xml:space="preserve">Global Parts</t>
+    <t xml:space="preserve">C7296801</t>
   </si>
   <si>
     <t xml:space="preserve">1x5 Female, Conn Rcpt,   SMD,  R/A, 2.54mm</t>
@@ -272,6 +272,9 @@
     <t xml:space="preserve">J3, J4</t>
   </si>
   <si>
+    <t xml:space="preserve">C21116902</t>
+  </si>
+  <si>
     <t xml:space="preserve">NPN/PNP Transistor Pair,  40V 0.2A </t>
   </si>
   <si>
@@ -281,6 +284,9 @@
     <t xml:space="preserve"> SOT-963</t>
   </si>
   <si>
+    <t xml:space="preserve">C896439</t>
+  </si>
+  <si>
     <t xml:space="preserve">W25Q16JVUXIQ TR, Serial Flash Memory, 16MBIT </t>
   </si>
   <si>
@@ -288,6 +294,9 @@
   </si>
   <si>
     <t xml:space="preserve">8-USON (2x3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C5333738</t>
   </si>
 </sst>
 </file>
@@ -527,7 +536,7 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1923,7 +1932,7 @@
         <v>65</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E20" s="1" t="n">
         <v>2</v>
@@ -1931,16 +1940,16 @@
     </row>
     <row r="21" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="E21" s="1" t="n">
         <v>34</v>
@@ -1950,16 +1959,16 @@
     </row>
     <row r="22" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="E22" s="1" t="n">
         <v>1</v>

</xml_diff>